<commit_message>
24 feb 2021 n
24 feb 2021 11:18 pM
</commit_message>
<xml_diff>
--- a/readme/Book1.xlsx
+++ b/readme/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A -1\Desktop\tr_au_fm\readme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\fyp\readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -65,6 +65,9 @@
     <t>table-name</t>
   </si>
   <si>
+    <t>createBY</t>
+  </si>
+  <si>
     <t>foreign</t>
   </si>
   <si>
@@ -77,23 +80,38 @@
     <t>agents</t>
   </si>
   <si>
+    <t>customers</t>
+  </si>
+  <si>
     <t>cnic</t>
   </si>
   <si>
+    <t>fathername</t>
+  </si>
+  <si>
     <t>profilepicture</t>
   </si>
   <si>
-    <t>createby</t>
-  </si>
-  <si>
-    <t>clients</t>
+    <t>visitorquery</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>auto_generated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,8 +172,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +213,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -207,22 +245,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -505,20 +546,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -529,21 +571,27 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -553,8 +601,11 @@
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -564,8 +615,11 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -573,32 +627,41 @@
         <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -606,76 +669,92 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>